<commit_message>
refactor file directory to distinguish different figure level , complete VW Figures mothods such as getPrecedingFigures and getFollowingFiguers which could be used for generating ballroom routines
</commit_message>
<xml_diff>
--- a/dancepose/src/main/resources/Ballroom/VW/NaturalTurn.xlsx
+++ b/dancepose/src/main/resources/Ballroom/VW/NaturalTurn.xlsx
@@ -4,40 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16420" activeTab="1"/>
+    <workbookView windowHeight="24260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAN" sheetId="1" r:id="rId1"/>
     <sheet name="LADY" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
-    <r>
-      <t>Step</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Source Sans Pro"/>
-        <charset val="134"/>
-      </rPr>
-      <t>_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FF666666"/>
-        <rFont val="Source Sans Pro"/>
-        <charset val="134"/>
-      </rPr>
-      <t>#</t>
-    </r>
+    <t>Step</t>
   </si>
   <si>
     <t>Steps</t>
@@ -195,12 +175,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,22 +189,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF666666"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF666666"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF1E1E1E"/>
+      <name val="Times New Roman Regular"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
-      <color rgb="FF666666"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF1E1E1E"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,6 +237,28 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,8 +272,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,37 +341,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -299,44 +349,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -344,35 +356,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -389,13 +378,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,168 +558,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -583,11 +572,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -596,22 +591,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,15 +607,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -680,177 +651,216 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1174,7 +1184,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C4" sqref="A1:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="6"/>
@@ -1182,240 +1192,241 @@
     <col min="2" max="2" width="17.7053571428571" customWidth="1"/>
     <col min="3" max="3" width="37.6428571428571" customWidth="1"/>
     <col min="4" max="4" width="15.9196428571429" customWidth="1"/>
+    <col min="5" max="5" width="14.8839285714286" customWidth="1"/>
     <col min="8" max="8" width="28.2767857142857" customWidth="1"/>
-    <col min="11" max="11" width="10.2678571428571" customWidth="1"/>
+    <col min="11" max="11" width="15.4821428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="39" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="6" customFormat="1" ht="33" spans="1:11">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="39" spans="1:11">
-      <c r="A2" s="3">
+    <row r="2" s="6" customFormat="1" spans="1:11">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="8">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" ht="58" spans="1:11">
-      <c r="A3" s="3">
+    <row r="3" s="6" customFormat="1" ht="33" spans="1:11">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="8">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="8"/>
+      <c r="J3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" ht="58" spans="1:11">
-      <c r="A4" s="3">
+    <row r="4" s="6" customFormat="1" spans="1:11">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="8">
         <v>3</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="I4" s="8"/>
+      <c r="J4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" ht="58" spans="1:11">
-      <c r="A5" s="3">
+    <row r="5" s="6" customFormat="1" spans="1:11">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="8"/>
+      <c r="K5" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" ht="116" spans="1:11">
-      <c r="A6" s="3">
+    <row r="6" s="6" customFormat="1" ht="33" spans="1:11">
+      <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="8">
         <v>2</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="8"/>
+      <c r="J6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" ht="58" spans="1:11">
-      <c r="A7" s="3">
+    <row r="7" s="6" customFormat="1" spans="1:11">
+      <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="8">
         <v>3</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1431,250 +1442,252 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="6"/>
   <cols>
+    <col min="1" max="1" width="9.14285714285714" style="3"/>
     <col min="2" max="2" width="20.6785714285714" customWidth="1"/>
     <col min="3" max="3" width="30.7946428571429" customWidth="1"/>
     <col min="4" max="4" width="17.7053571428571" customWidth="1"/>
+    <col min="5" max="5" width="15.4732142857143" customWidth="1"/>
     <col min="7" max="7" width="14.5714285714286" customWidth="1"/>
-    <col min="8" max="8" width="22.3125" customWidth="1"/>
+    <col min="8" max="8" width="24.0982142857143" customWidth="1"/>
     <col min="10" max="10" width="17.1071428571429" customWidth="1"/>
     <col min="11" max="11" width="19.7857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="39" spans="1:11">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="1" ht="17" spans="1:11">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="39" spans="1:11">
-      <c r="A2" s="3">
+    <row r="2" s="2" customFormat="1" ht="17" spans="1:11">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" ht="116" spans="1:11">
-      <c r="A3" s="3">
+    <row r="3" s="2" customFormat="1" ht="33" spans="1:11">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" ht="58" spans="1:11">
-      <c r="A4" s="3">
+    <row r="4" s="2" customFormat="1" ht="17" spans="1:11">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>3</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" ht="58" spans="1:11">
-      <c r="A5" s="3">
+    <row r="5" s="2" customFormat="1" ht="17" spans="1:11">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>1</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" ht="58" spans="1:11">
-      <c r="A6" s="3">
+    <row r="6" s="2" customFormat="1" ht="17" spans="1:11">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>2</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" ht="58" spans="1:11">
-      <c r="A7" s="3">
+    <row r="7" s="2" customFormat="1" ht="17" spans="1:11">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>3</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="K7" s="5" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>